<commit_message>
week 2 in progress
</commit_message>
<xml_diff>
--- a/clojure-projects/src/ica/data.xlsx
+++ b/clojure-projects/src/ica/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leonov\PCU\SymbolicComputation2024\clojure-projects\src\clojure_projects\ica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leonov\PCU\SymbolicComputation2404\clojure-projects\src\ica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27324917-979F-4867-AC5A-533FBD4C23E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51572975-721F-4366-98A8-C47678AC6F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BFB9042F-2CAF-4781-AD5D-9F737D043F14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BFB9042F-2CAF-4781-AD5D-9F737D043F14}"/>
   </bookViews>
   <sheets>
     <sheet name="Team1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="35">
   <si>
     <t>City</t>
   </si>
@@ -132,6 +132,18 @@
   </si>
   <si>
     <t>Truck Number</t>
+  </si>
+  <si>
+    <t>Kory David DeJong</t>
+  </si>
+  <si>
+    <t>Matvii Kharchenko</t>
+  </si>
+  <si>
+    <t>Divan Wayne Ingram</t>
+  </si>
+  <si>
+    <t>Burak Ugar</t>
   </si>
 </sst>
 </file>
@@ -717,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D4F94F-961B-4669-90C3-16E30A1031FB}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,6 +739,7 @@
     <col min="3" max="3" width="16.5546875" customWidth="1"/>
     <col min="4" max="5" width="15.21875" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -772,6 +785,9 @@
       <c r="F2">
         <v>3</v>
       </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -786,6 +802,9 @@
       <c r="D3">
         <v>200</v>
       </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -800,6 +819,9 @@
       <c r="D4">
         <v>100</v>
       </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -813,6 +835,9 @@
       </c>
       <c r="D5">
         <v>80</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1092,7 +1117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1092226F-A661-4783-85A9-DD530D81C1ED}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>